<commit_message>
add write and read data-fles
</commit_message>
<xml_diff>
--- a/files/log.xlsx
+++ b/files/log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>аплікатор</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>опис дій / заміни запчастин</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>Gamma 1 (8_1235)</t>
@@ -64,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,9 +236,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Добре" xfId="1" builtinId="26"/>
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
     <cellStyle name="Звичайний 3" xfId="2"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -256,7 +253,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартна">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -294,7 +291,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартна">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -328,7 +325,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -363,10 +359,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартна">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -539,14 +534,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
@@ -557,7 +552,7 @@
     <col min="8" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="6"/>
       <c r="B1" s="7"/>
       <c r="C1" s="8"/>
@@ -566,7 +561,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -589,64 +584,64 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>43103.636886574073</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="11">
         <v>10</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>43103.636886574073</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>7</v>
+      <c r="B4" s="10">
+        <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="10"/>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>43103.636886574073</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>7</v>
+      <c r="B5" s="10">
+        <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11">
         <v>20</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="13"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="15" t="s">
-        <v>14</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="D6" s="16"/>
     </row>

</xml_diff>

<commit_message>
add write data to files
</commit_message>
<xml_diff>
--- a/files/log.xlsx
+++ b/files/log.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+  <si>
+    <t>дата, час</t>
+  </si>
+  <si>
+    <t>зміна</t>
+  </si>
+  <si>
+    <t>обладнання</t>
+  </si>
   <si>
     <t>аплікатор</t>
   </si>
   <si>
-    <t>дата, час</t>
-  </si>
-  <si>
-    <t>зміна</t>
-  </si>
-  <si>
-    <t>обладнання</t>
-  </si>
-  <si>
     <t>витрачений час, хв.</t>
   </si>
   <si>
@@ -53,6 +53,36 @@
   </si>
   <si>
     <t>очікування налагоджувача</t>
+  </si>
+  <si>
+    <t>18/06/2018</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>проблеми з матеріалом</t>
+  </si>
+  <si>
+    <t>test of sum</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>**</t>
@@ -62,43 +92,44 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
       <sz val="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -110,7 +141,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.3999755851924192"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,69 +215,64 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="18">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="26" name="Хороший" xfId="1"/>
     <cellStyle name="Звичайний 3" xfId="2"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -534,45 +560,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.28515625" customWidth="1"/>
-    <col min="7" max="7" width="51" customWidth="1"/>
-    <col min="8" max="9" width="9" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="10.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="4" min="3" width="23"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="17" width="11.7109375"/>
+    <col customWidth="1" max="6" min="6" width="41.28515625"/>
+    <col customWidth="1" max="7" min="7" width="51"/>
+    <col customWidth="1" max="9" min="8" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="30">
+    <row customHeight="1" ht="21" r="1" spans="1:7">
+      <c r="A1" s="6" t="n"/>
+      <c r="B1" s="7" t="n"/>
+      <c r="C1" s="8" t="n"/>
+      <c r="D1" s="8" t="n"/>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="8" t="n"/>
+      <c r="G1" s="14" t="n"/>
+    </row>
+    <row customHeight="1" ht="30" r="2" spans="1:7">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
@@ -585,17 +615,17 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>43103.636886574073</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="A3" s="1" t="n">
+        <v>43103.63688657407</v>
+      </c>
+      <c r="B3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11">
+      <c r="D3" s="10" t="n"/>
+      <c r="E3" s="11" t="n">
         <v>10</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -606,46 +636,918 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>43103.636886574073</v>
-      </c>
-      <c r="B4" s="10">
+      <c r="A4" s="1" t="n">
+        <v>43103.63688657407</v>
+      </c>
+      <c r="B4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="13"/>
+      <c r="D4" s="10" t="n"/>
+      <c r="E4" s="11" t="n"/>
+      <c r="F4" s="10" t="n"/>
+      <c r="G4" s="13" t="n"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>43103.636886574073</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="1" t="n">
+        <v>43103.63688657407</v>
+      </c>
+      <c r="B5" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11">
+      <c r="D5" s="10" t="n"/>
+      <c r="E5" s="11" t="n">
         <v>20</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="13"/>
+      <c r="G5" s="13" t="n"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="16" t="n"/>
+      <c r="E6" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1111</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E15" t="n">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E20" t="n">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E22" t="n">
+        <v>111</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E23" t="n">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E29" t="n">
+        <v>480</v>
+      </c>
+      <c r="F29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E30" t="n">
+        <v>480</v>
+      </c>
+      <c r="F30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E31" t="n">
+        <v>480</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E33" t="n">
+        <v>480</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E34" t="n">
+        <v>500</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E35" t="n">
+        <v>900</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E36" t="n">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="n">
+        <v>80001840</v>
+      </c>
+      <c r="E37" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="n">
+        <v>80001840</v>
+      </c>
+      <c r="E38" t="n">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="n">
+        <v>80001</v>
+      </c>
+      <c r="E39" t="n">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="n">
+        <v>800011</v>
+      </c>
+      <c r="E40" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E41" t="n">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E42" t="n">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E43" t="n">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E44" t="n">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E45" t="n">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E46" t="n">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E47" t="n">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E48" t="n">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E49" t="n">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D50" t="s"/>
+      <c r="E50" t="n">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add check input number, but not apl
</commit_message>
<xml_diff>
--- a/files/log.xlsx
+++ b/files/log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>дата, час</t>
   </si>
@@ -76,13 +76,52 @@
     <t>проблеми з матеріалом</t>
   </si>
   <si>
-    <t>test of sum</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>20/06/2018</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>11</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>0231</t>
+  </si>
+  <si>
+    <t>0571</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>80001234</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>8000123</t>
+  </si>
+  <si>
+    <t>123i</t>
+  </si>
+  <si>
+    <t>80001</t>
+  </si>
+  <si>
+    <t>21/06/2018</t>
   </si>
   <si>
     <t>**</t>
@@ -565,10 +604,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -777,13 +816,16 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="C12" t="n">
+        <v>80001841</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -794,16 +836,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C13" t="n">
         <v>80001841</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>480</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -814,16 +856,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14" t="n">
         <v>80001841</v>
       </c>
       <c r="E14" t="n">
-        <v>1111</v>
+        <v>500</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
@@ -840,10 +882,10 @@
         <v>80001841</v>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
@@ -854,16 +896,16 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n">
         <v>80001841</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
@@ -877,13 +919,13 @@
         <v>18</v>
       </c>
       <c r="C17" t="n">
-        <v>80001841</v>
+        <v>80001840</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
@@ -894,16 +936,16 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C18" t="n">
-        <v>80001841</v>
+        <v>80001840</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
@@ -917,16 +959,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>80001841</v>
+        <v>80001</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -934,44 +973,41 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>80001841</v>
+        <v>800011</v>
       </c>
       <c r="E20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C21" t="n">
-        <v>80001841</v>
+        <v>8000184</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -980,18 +1016,18 @@
         <v>80001841</v>
       </c>
       <c r="E22" t="n">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -1000,18 +1036,18 @@
         <v>80001841</v>
       </c>
       <c r="E23" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -1020,18 +1056,18 @@
         <v>80001841</v>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -1039,19 +1075,22 @@
       <c r="C25" t="n">
         <v>80001841</v>
       </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
       <c r="E25" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
@@ -1059,19 +1098,19 @@
       <c r="C26" t="n">
         <v>80001841</v>
       </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
       <c r="E26" t="n">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
@@ -1079,16 +1118,22 @@
       <c r="C27" t="n">
         <v>80001841</v>
       </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
@@ -1096,31 +1141,37 @@
       <c r="C28" t="n">
         <v>80001841</v>
       </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C29" t="n">
         <v>80001841</v>
       </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
       <c r="E29" t="n">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G29" t="s">
         <v>16</v>
@@ -1128,7 +1179,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
@@ -1136,19 +1187,22 @@
       <c r="C30" t="n">
         <v>80001841</v>
       </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
       <c r="E30" t="n">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
@@ -1156,19 +1210,22 @@
       <c r="C31" t="n">
         <v>80001841</v>
       </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
       <c r="E31" t="n">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
@@ -1177,18 +1234,18 @@
         <v>80001841</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
@@ -1196,19 +1253,22 @@
       <c r="C33" t="n">
         <v>80001841</v>
       </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
       <c r="E33" t="n">
-        <v>480</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -1216,19 +1276,22 @@
       <c r="C34" t="n">
         <v>80001841</v>
       </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
       <c r="E34" t="n">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B35" t="s">
         <v>18</v>
@@ -1237,10 +1300,10 @@
         <v>80001841</v>
       </c>
       <c r="E35" t="n">
-        <v>900</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G35" t="s">
         <v>16</v>
@@ -1248,7 +1311,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -1257,92 +1320,95 @@
         <v>80001841</v>
       </c>
       <c r="E36" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
       </c>
       <c r="C37" t="n">
-        <v>80001840</v>
+        <v>80001841</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
       </c>
       <c r="C38" t="n">
-        <v>80001840</v>
+        <v>80001841</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
         <v>18</v>
       </c>
       <c r="C39" t="n">
-        <v>80001</v>
+        <v>80001841</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
         <v>18</v>
       </c>
       <c r="C40" t="n">
-        <v>800011</v>
+        <v>80001841</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
       </c>
       <c r="E40" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
@@ -1350,19 +1416,19 @@
       <c r="C41" t="n">
         <v>80001841</v>
       </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
       <c r="E41" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>18</v>
@@ -1370,19 +1436,19 @@
       <c r="C42" t="n">
         <v>80001841</v>
       </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
       <c r="E42" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
         <v>18</v>
@@ -1391,18 +1457,15 @@
         <v>80001841</v>
       </c>
       <c r="E43" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
@@ -1411,18 +1474,18 @@
         <v>80001841</v>
       </c>
       <c r="E44" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
@@ -1430,19 +1493,22 @@
       <c r="C45" t="n">
         <v>80001841</v>
       </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
       <c r="E45" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
         <v>18</v>
@@ -1450,19 +1516,22 @@
       <c r="C46" t="n">
         <v>80001841</v>
       </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
       <c r="E46" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -1470,19 +1539,22 @@
       <c r="C47" t="n">
         <v>80001841</v>
       </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
       <c r="E47" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G47" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -1491,59 +1563,434 @@
         <v>80001841</v>
       </c>
       <c r="E48" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C49" t="n">
         <v>80001841</v>
       </c>
+      <c r="D49" t="s">
+        <v>32</v>
+      </c>
       <c r="E49" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C50" t="n">
         <v>80001841</v>
       </c>
-      <c r="D50" t="s"/>
+      <c r="D50" t="s">
+        <v>33</v>
+      </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G50" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D54" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D65" t="s">
+        <v>32</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D66" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D67" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="n">
+        <v>80001841</v>
+      </c>
+      <c r="D68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="s"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>